<commit_message>
add withdrawalMethode and some feedback changes
</commit_message>
<xml_diff>
--- a/controllers/exports/categories.xlsx
+++ b/controllers/exports/categories.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -417,13 +417,13 @@
         <v>logo</v>
       </c>
       <c r="E1" t="str">
-        <v>isActive</v>
+        <v>createdAt</v>
       </c>
       <c r="F1" t="str">
-        <v>createdAt</v>
+        <v>updatedAt</v>
       </c>
       <c r="G1" t="str">
-        <v>updatedAt</v>
+        <v>status</v>
       </c>
     </row>
     <row r="2">
@@ -439,14 +439,14 @@
       <c r="D2" t="str">
         <v>https://res.cloudinary.com/dgexhjryd/image/upload/v1729082555/Lailoji/logo-1729082551627.jpg</v>
       </c>
-      <c r="E2" t="str">
-        <v>active</v>
+      <c r="E2" s="1">
+        <v>45581.75886135417</v>
       </c>
       <c r="F2" s="1">
-        <v>45581.75886135417</v>
-      </c>
-      <c r="G2" s="1">
-        <v>45581.75994142361</v>
+        <v>45584.72708806713</v>
+      </c>
+      <c r="G2" t="str">
+        <v>Active</v>
       </c>
     </row>
     <row r="3">
@@ -462,42 +462,203 @@
       <c r="D3" t="str">
         <v>https://res.cloudinary.com/dgexhjryd/image/upload/v1729082727/Lailoji/logo-1729082723749.jpg</v>
       </c>
-      <c r="E3" t="str">
-        <v>active</v>
+      <c r="E3" s="1">
+        <v>45581.76085006945</v>
       </c>
       <c r="F3" s="1">
-        <v>45581.76085006945</v>
-      </c>
-      <c r="G3" s="1">
-        <v>45581.76085006945</v>
+        <v>45584.508307986114</v>
+      </c>
+      <c r="G3" t="str">
+        <v>Active</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>6710b1a78655485fbf55c96a</v>
+        <v>6719f2bb49e1f74e65127577</v>
       </c>
       <c r="B4" t="str">
-        <v>Cloths</v>
+        <v>Furniture</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4" t="str">
-        <v>https://res.cloudinary.com/dgexhjryd/image/upload/v1729147304/Lailoji/logo-1729147298813.jpg</v>
-      </c>
-      <c r="E4" t="str">
-        <v>active</v>
+        <v>https://res.cloudinary.com/dgexhjryd/image/upload/v1729753811/Lailoji/logo-1729753810993.jpg</v>
+      </c>
+      <c r="E4" s="1">
+        <v>45589.52774784722</v>
       </c>
       <c r="F4" s="1">
-        <v>45582.50825436343</v>
-      </c>
-      <c r="G4" s="1">
-        <v>45582.50842478009</v>
+        <v>45589.52831390046</v>
+      </c>
+      <c r="G4" t="str">
+        <v>Inactive</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>671b2a00e944f0b5198daf9a</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Handbags</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" t="str">
+        <v>https://res.cloudinary.com/dgexhjryd/image/upload/v1729082555/Lailoji/logo-1729082551627.jpg</v>
+      </c>
+      <c r="E5" s="1">
+        <v>45590.45002712963</v>
+      </c>
+      <c r="F5" s="1">
+        <v>45590.45002712963</v>
+      </c>
+      <c r="G5" t="str">
+        <v>Inactive</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>671b2a00e944f0b5198daf9b</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Shoes</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="str">
+        <v>https://res.cloudinary.com/dgexhjryd/image/upload/v1729082555/Lailoji/logo-1729082551627.jpg</v>
+      </c>
+      <c r="E6" s="1">
+        <v>45590.45002712963</v>
+      </c>
+      <c r="F6" s="1">
+        <v>45590.45002712963</v>
+      </c>
+      <c r="G6" t="str">
+        <v>Inactive</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>6729ac9fbe93e05ec4836723</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Garden</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="str">
+        <v>https://res.cloudinary.com/dgexhjryd/image/upload/v1730784463/Lailoji/logo-1730784463444.jpg</v>
+      </c>
+      <c r="E7" s="1">
+        <v>45601.45631443287</v>
+      </c>
+      <c r="F7" s="1">
+        <v>45601.45687869213</v>
+      </c>
+      <c r="G7" t="str">
+        <v>Inactive</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>6729b3472ea45155a9a73ffb</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Electronics</v>
+      </c>
+      <c r="C8" t="str">
+        <v>high</v>
+      </c>
+      <c r="D8" t="str">
+        <v>https://res.cloudinary.com/dgexhjryd/image/upload/v1730786356/Lailoji/logo-1730786353820.jpg</v>
+      </c>
+      <c r="E8" s="1">
+        <v>45601.47604179398</v>
+      </c>
+      <c r="F8" s="1">
+        <v>45601.47881064815</v>
+      </c>
+      <c r="G8" t="str">
+        <v>Inactive</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>6729bbcf8ac6688c38353ce9</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Medicine</v>
+      </c>
+      <c r="C9" t="str">
+        <v>low</v>
+      </c>
+      <c r="D9" t="str">
+        <v>https://res.cloudinary.com/dgexhjryd/image/upload/v1730788301/Lailoji/logo-1730788300510.jpg</v>
+      </c>
+      <c r="E9" s="1">
+        <v>45601.501319375</v>
+      </c>
+      <c r="F9" s="1">
+        <v>45601.501319375</v>
+      </c>
+      <c r="G9" t="str">
+        <v>Inactive</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>6729bc308ac6688c38353cec</v>
+      </c>
+      <c r="B10" t="str">
+        <v>gif</v>
+      </c>
+      <c r="C10" t="str">
+        <v>low</v>
+      </c>
+      <c r="D10" t="str">
+        <v>https://res.cloudinary.com/dgexhjryd/image/upload/v1730788398/Lailoji/logo-1730788397696.gif</v>
+      </c>
+      <c r="E10" s="1">
+        <v>45601.50244056713</v>
+      </c>
+      <c r="F10" s="1">
+        <v>45601.50244056713</v>
+      </c>
+      <c r="G10" t="str">
+        <v>Inactive</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>6729be8d8ac6688c38353cfd</v>
+      </c>
+      <c r="B11" t="str">
+        <v>Fruits</v>
+      </c>
+      <c r="C11" t="str">
+        <v>low</v>
+      </c>
+      <c r="D11" t="str">
+        <v>https://res.cloudinary.com/dgexhjryd/image/upload/v1730789069/Lailoji/logo-1730789069069.jpg</v>
+      </c>
+      <c r="E11" s="1">
+        <v>45601.50943373843</v>
+      </c>
+      <c r="F11" s="1">
+        <v>45601.5102078125</v>
+      </c>
+      <c r="G11" t="str">
+        <v>Inactive</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G11"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>